<commit_message>
create a local cron to update data
</commit_message>
<xml_diff>
--- a/data/matches.xlsx
+++ b/data/matches.xlsx
@@ -760,7 +760,7 @@
         <v>5474</v>
       </c>
       <c r="K6" s="2" t="n">
-        <v>45395</v>
+        <v>45396</v>
       </c>
       <c r="L6" t="inlineStr">
         <is>
@@ -813,7 +813,7 @@
         <v>784663</v>
       </c>
       <c r="K7" s="2" t="n">
-        <v>45395</v>
+        <v>45396</v>
       </c>
       <c r="L7" t="inlineStr">
         <is>
@@ -866,7 +866,7 @@
         <v>784886</v>
       </c>
       <c r="K8" s="2" t="n">
-        <v>45395</v>
+        <v>45396</v>
       </c>
       <c r="L8" t="inlineStr">
         <is>
@@ -919,7 +919,7 @@
         <v>787598</v>
       </c>
       <c r="K9" s="2" t="n">
-        <v>45395</v>
+        <v>45396</v>
       </c>
       <c r="L9" t="inlineStr">
         <is>
@@ -972,7 +972,7 @@
         <v>794590</v>
       </c>
       <c r="K10" s="2" t="n">
-        <v>45395</v>
+        <v>45396</v>
       </c>
       <c r="L10" t="inlineStr">
         <is>
@@ -1025,7 +1025,7 @@
         <v>784709</v>
       </c>
       <c r="K11" s="2" t="n">
-        <v>45395</v>
+        <v>45396</v>
       </c>
       <c r="L11" t="inlineStr">
         <is>
@@ -1078,7 +1078,7 @@
         <v>108391</v>
       </c>
       <c r="K12" s="2" t="n">
-        <v>45395</v>
+        <v>45398</v>
       </c>
       <c r="L12" t="inlineStr">
         <is>
@@ -1174,7 +1174,7 @@
         <v>798839</v>
       </c>
       <c r="K14" s="2" t="n">
-        <v>45395</v>
+        <v>45399</v>
       </c>
       <c r="L14" t="inlineStr">
         <is>
@@ -1227,7 +1227,7 @@
         <v>804981</v>
       </c>
       <c r="K15" s="2" t="n">
-        <v>45395</v>
+        <v>45399</v>
       </c>
       <c r="L15" t="inlineStr">
         <is>
@@ -1280,7 +1280,7 @@
         <v>791416</v>
       </c>
       <c r="K16" s="2" t="n">
-        <v>45395</v>
+        <v>45399</v>
       </c>
       <c r="L16" t="inlineStr">
         <is>
@@ -1333,7 +1333,7 @@
         <v>801563</v>
       </c>
       <c r="K17" s="2" t="n">
-        <v>45395</v>
+        <v>45399</v>
       </c>
       <c r="L17" t="inlineStr">
         <is>
@@ -1386,7 +1386,7 @@
         <v>802281</v>
       </c>
       <c r="K18" s="2" t="n">
-        <v>45395</v>
+        <v>45399</v>
       </c>
       <c r="L18" t="inlineStr">
         <is>
@@ -1439,7 +1439,7 @@
         <v>784639</v>
       </c>
       <c r="K19" s="2" t="n">
-        <v>45395</v>
+        <v>45399</v>
       </c>
       <c r="L19" t="inlineStr">
         <is>
@@ -1492,7 +1492,7 @@
         <v>785466</v>
       </c>
       <c r="K20" s="2" t="n">
-        <v>45395</v>
+        <v>45399</v>
       </c>
       <c r="L20" t="inlineStr">
         <is>
@@ -1545,7 +1545,7 @@
         <v>797117</v>
       </c>
       <c r="K21" s="2" t="n">
-        <v>45395</v>
+        <v>45400</v>
       </c>
       <c r="L21" t="inlineStr">
         <is>
@@ -1598,7 +1598,7 @@
         <v>793051</v>
       </c>
       <c r="K22" s="2" t="n">
-        <v>45395</v>
+        <v>45448</v>
       </c>
       <c r="L22" t="inlineStr">
         <is>
@@ -1694,7 +1694,7 @@
         <v>804981</v>
       </c>
       <c r="K24" s="2" t="n">
-        <v>45395</v>
+        <v>45402</v>
       </c>
       <c r="L24" t="inlineStr">
         <is>
@@ -1747,7 +1747,7 @@
         <v>5474</v>
       </c>
       <c r="K25" s="2" t="n">
-        <v>45395</v>
+        <v>45402</v>
       </c>
       <c r="L25" t="inlineStr">
         <is>
@@ -1800,7 +1800,7 @@
         <v>802281</v>
       </c>
       <c r="K26" s="2" t="n">
-        <v>45395</v>
+        <v>45402</v>
       </c>
       <c r="L26" t="inlineStr">
         <is>
@@ -1853,7 +1853,7 @@
         <v>801563</v>
       </c>
       <c r="K27" s="2" t="n">
-        <v>45395</v>
+        <v>45402</v>
       </c>
       <c r="L27" t="inlineStr">
         <is>
@@ -1906,7 +1906,7 @@
         <v>784639</v>
       </c>
       <c r="K28" s="2" t="n">
-        <v>45395</v>
+        <v>45403</v>
       </c>
       <c r="L28" t="inlineStr">
         <is>
@@ -1959,7 +1959,7 @@
         <v>784663</v>
       </c>
       <c r="K29" s="2" t="n">
-        <v>45395</v>
+        <v>45403</v>
       </c>
       <c r="L29" t="inlineStr">
         <is>
@@ -2012,7 +2012,7 @@
         <v>787735</v>
       </c>
       <c r="K30" s="2" t="n">
-        <v>45395</v>
+        <v>45403</v>
       </c>
       <c r="L30" t="inlineStr">
         <is>
@@ -2065,7 +2065,7 @@
         <v>785466</v>
       </c>
       <c r="K31" s="2" t="n">
-        <v>45395</v>
+        <v>45403</v>
       </c>
       <c r="L31" t="inlineStr">
         <is>
@@ -2118,7 +2118,7 @@
         <v>784982</v>
       </c>
       <c r="K32" s="2" t="n">
-        <v>45395</v>
+        <v>45403</v>
       </c>
       <c r="L32" t="inlineStr">
         <is>
@@ -2214,7 +2214,7 @@
         <v>791416</v>
       </c>
       <c r="K34" s="2" t="n">
-        <v>45395</v>
+        <v>45409</v>
       </c>
       <c r="L34" t="inlineStr">
         <is>
@@ -2267,7 +2267,7 @@
         <v>784886</v>
       </c>
       <c r="K35" s="2" t="n">
-        <v>45395</v>
+        <v>45409</v>
       </c>
       <c r="L35" t="inlineStr">
         <is>
@@ -2320,7 +2320,7 @@
         <v>787598</v>
       </c>
       <c r="K36" s="2" t="n">
-        <v>45395</v>
+        <v>45409</v>
       </c>
       <c r="L36" t="inlineStr">
         <is>
@@ -2373,7 +2373,7 @@
         <v>794590</v>
       </c>
       <c r="K37" s="2" t="n">
-        <v>45395</v>
+        <v>45410</v>
       </c>
       <c r="L37" t="inlineStr">
         <is>
@@ -2426,7 +2426,7 @@
         <v>108391</v>
       </c>
       <c r="K38" s="2" t="n">
-        <v>45395</v>
+        <v>45410</v>
       </c>
       <c r="L38" t="inlineStr">
         <is>
@@ -2479,7 +2479,7 @@
         <v>793051</v>
       </c>
       <c r="K39" s="2" t="n">
-        <v>45395</v>
+        <v>45410</v>
       </c>
       <c r="L39" t="inlineStr">
         <is>
@@ -2532,7 +2532,7 @@
         <v>125341</v>
       </c>
       <c r="K40" s="2" t="n">
-        <v>45395</v>
+        <v>45410</v>
       </c>
       <c r="L40" t="inlineStr">
         <is>
@@ -2585,7 +2585,7 @@
         <v>798839</v>
       </c>
       <c r="K41" s="2" t="n">
-        <v>45395</v>
+        <v>45410</v>
       </c>
       <c r="L41" t="inlineStr">
         <is>
@@ -2638,7 +2638,7 @@
         <v>797117</v>
       </c>
       <c r="K42" s="2" t="n">
-        <v>45395</v>
+        <v>45410</v>
       </c>
       <c r="L42" t="inlineStr">
         <is>
@@ -2691,7 +2691,7 @@
         <v>784709</v>
       </c>
       <c r="K43" s="2" t="n">
-        <v>45395</v>
+        <v>45411</v>
       </c>
       <c r="L43" t="inlineStr">
         <is>
@@ -2744,7 +2744,7 @@
         <v>784886</v>
       </c>
       <c r="K44" s="2" t="n">
-        <v>45395</v>
+        <v>45416</v>
       </c>
       <c r="L44" t="inlineStr">
         <is>
@@ -2797,7 +2797,7 @@
         <v>784663</v>
       </c>
       <c r="K45" s="2" t="n">
-        <v>45395</v>
+        <v>45416</v>
       </c>
       <c r="L45" t="inlineStr">
         <is>
@@ -2850,7 +2850,7 @@
         <v>786600</v>
       </c>
       <c r="K46" s="2" t="n">
-        <v>45395</v>
+        <v>45416</v>
       </c>
       <c r="L46" t="inlineStr">
         <is>
@@ -2903,7 +2903,7 @@
         <v>804981</v>
       </c>
       <c r="K47" s="2" t="n">
-        <v>45395</v>
+        <v>45417</v>
       </c>
       <c r="L47" t="inlineStr">
         <is>
@@ -2956,7 +2956,7 @@
         <v>785466</v>
       </c>
       <c r="K48" s="2" t="n">
-        <v>45395</v>
+        <v>45417</v>
       </c>
       <c r="L48" t="inlineStr">
         <is>
@@ -3009,7 +3009,7 @@
         <v>787735</v>
       </c>
       <c r="K49" s="2" t="n">
-        <v>45395</v>
+        <v>45417</v>
       </c>
       <c r="L49" t="inlineStr">
         <is>
@@ -3062,7 +3062,7 @@
         <v>784709</v>
       </c>
       <c r="K50" s="2" t="n">
-        <v>45395</v>
+        <v>45417</v>
       </c>
       <c r="L50" t="inlineStr">
         <is>
@@ -3115,7 +3115,7 @@
         <v>797117</v>
       </c>
       <c r="K51" s="2" t="n">
-        <v>45395</v>
+        <v>45448</v>
       </c>
       <c r="L51" t="inlineStr">
         <is>
@@ -3168,7 +3168,7 @@
         <v>802281</v>
       </c>
       <c r="K52" s="2" t="n">
-        <v>45395</v>
+        <v>45423</v>
       </c>
       <c r="L52" t="inlineStr">
         <is>
@@ -3221,7 +3221,7 @@
         <v>801563</v>
       </c>
       <c r="K53" s="2" t="n">
-        <v>45395</v>
+        <v>45424</v>
       </c>
       <c r="L53" t="inlineStr">
         <is>
@@ -3274,7 +3274,7 @@
         <v>794590</v>
       </c>
       <c r="K54" s="2" t="n">
-        <v>45395</v>
+        <v>45424</v>
       </c>
       <c r="L54" t="inlineStr">
         <is>
@@ -3327,7 +3327,7 @@
         <v>798839</v>
       </c>
       <c r="K55" s="2" t="n">
-        <v>45395</v>
+        <v>45424</v>
       </c>
       <c r="L55" t="inlineStr">
         <is>
@@ -3380,7 +3380,7 @@
         <v>125341</v>
       </c>
       <c r="K56" s="2" t="n">
-        <v>45395</v>
+        <v>45424</v>
       </c>
       <c r="L56" t="inlineStr">
         <is>
@@ -3433,7 +3433,7 @@
         <v>793051</v>
       </c>
       <c r="K57" s="2" t="n">
-        <v>45395</v>
+        <v>45424</v>
       </c>
       <c r="L57" t="inlineStr">
         <is>
@@ -3486,7 +3486,7 @@
         <v>108391</v>
       </c>
       <c r="K58" s="2" t="n">
-        <v>45395</v>
+        <v>45425</v>
       </c>
       <c r="L58" t="inlineStr">
         <is>
@@ -3539,7 +3539,7 @@
         <v>5474</v>
       </c>
       <c r="K59" s="2" t="n">
-        <v>45395</v>
+        <v>45452</v>
       </c>
       <c r="L59" t="inlineStr">
         <is>
@@ -3592,7 +3592,7 @@
         <v>125341</v>
       </c>
       <c r="K60" s="2" t="n">
-        <v>45395</v>
+        <v>45444</v>
       </c>
       <c r="L60" t="inlineStr">
         <is>
@@ -3645,7 +3645,7 @@
         <v>164969</v>
       </c>
       <c r="K61" s="2" t="n">
-        <v>45395</v>
+        <v>45444</v>
       </c>
       <c r="L61" t="inlineStr">
         <is>
@@ -3698,7 +3698,7 @@
         <v>784639</v>
       </c>
       <c r="K62" s="2" t="n">
-        <v>45395</v>
+        <v>45444</v>
       </c>
       <c r="L62" t="inlineStr">
         <is>
@@ -3751,7 +3751,7 @@
         <v>784982</v>
       </c>
       <c r="K63" s="2" t="n">
-        <v>45395</v>
+        <v>45444</v>
       </c>
       <c r="L63" t="inlineStr">
         <is>
@@ -3804,7 +3804,7 @@
         <v>794590</v>
       </c>
       <c r="K64" s="2" t="n">
-        <v>45395</v>
+        <v>45444</v>
       </c>
       <c r="L64" t="inlineStr">
         <is>
@@ -3857,7 +3857,7 @@
         <v>787735</v>
       </c>
       <c r="K65" s="2" t="n">
-        <v>45395</v>
+        <v>45445</v>
       </c>
       <c r="L65" t="inlineStr">
         <is>
@@ -3910,7 +3910,7 @@
         <v>784709</v>
       </c>
       <c r="K66" s="2" t="n">
-        <v>45395</v>
+        <v>45445</v>
       </c>
       <c r="L66" t="inlineStr">
         <is>
@@ -3963,7 +3963,7 @@
         <v>784663</v>
       </c>
       <c r="K67" s="2" t="n">
-        <v>45395</v>
+        <v>45445</v>
       </c>
       <c r="L67" t="inlineStr">
         <is>
@@ -4016,7 +4016,7 @@
         <v>798839</v>
       </c>
       <c r="K68" s="2" t="n">
-        <v>45395</v>
+        <v>45445</v>
       </c>
       <c r="L68" t="inlineStr">
         <is>
@@ -4069,7 +4069,7 @@
         <v>801563</v>
       </c>
       <c r="K69" s="2" t="n">
-        <v>45395</v>
+        <v>45445</v>
       </c>
       <c r="L69" t="inlineStr">
         <is>
@@ -4122,7 +4122,7 @@
         <v>802281</v>
       </c>
       <c r="K70" s="2" t="n">
-        <v>45395</v>
+        <v>45454</v>
       </c>
       <c r="L70" t="inlineStr">
         <is>
@@ -4175,7 +4175,7 @@
         <v>793051</v>
       </c>
       <c r="K71" s="2" t="n">
-        <v>45395</v>
+        <v>45454</v>
       </c>
       <c r="L71" t="inlineStr">
         <is>
@@ -4228,7 +4228,7 @@
         <v>108391</v>
       </c>
       <c r="K72" s="2" t="n">
-        <v>45395</v>
+        <v>45454</v>
       </c>
       <c r="L72" t="inlineStr">
         <is>
@@ -4281,7 +4281,7 @@
         <v>784886</v>
       </c>
       <c r="K73" s="2" t="n">
-        <v>45395</v>
+        <v>45454</v>
       </c>
       <c r="L73" t="inlineStr">
         <is>
@@ -4334,7 +4334,7 @@
         <v>5474</v>
       </c>
       <c r="K74" s="2" t="n">
-        <v>45395</v>
+        <v>45456</v>
       </c>
       <c r="L74" t="inlineStr">
         <is>
@@ -4387,7 +4387,7 @@
         <v>791416</v>
       </c>
       <c r="K75" s="2" t="n">
-        <v>45395</v>
+        <v>45456</v>
       </c>
       <c r="L75" t="inlineStr">
         <is>
@@ -4440,7 +4440,7 @@
         <v>787598</v>
       </c>
       <c r="K76" s="2" t="n">
-        <v>45395</v>
+        <v>45456</v>
       </c>
       <c r="L76" t="inlineStr">
         <is>
@@ -4493,7 +4493,7 @@
         <v>785466</v>
       </c>
       <c r="K77" s="2" t="n">
-        <v>45395</v>
+        <v>45456</v>
       </c>
       <c r="L77" t="inlineStr">
         <is>
@@ -4546,7 +4546,7 @@
         <v>786600</v>
       </c>
       <c r="K78" s="2" t="n">
-        <v>45395</v>
+        <v>45456</v>
       </c>
       <c r="L78" t="inlineStr">
         <is>
@@ -4599,7 +4599,7 @@
         <v>804981</v>
       </c>
       <c r="K79" s="2" t="n">
-        <v>45395</v>
+        <v>45456</v>
       </c>
       <c r="L79" t="inlineStr">
         <is>
@@ -4652,7 +4652,7 @@
         <v>784982</v>
       </c>
       <c r="K80" s="2" t="n">
-        <v>45395</v>
+        <v>45458</v>
       </c>
       <c r="L80" t="inlineStr">
         <is>
@@ -4705,7 +4705,7 @@
         <v>797117</v>
       </c>
       <c r="K81" s="2" t="n">
-        <v>45395</v>
+        <v>45458</v>
       </c>
       <c r="L81" t="inlineStr">
         <is>
@@ -4758,7 +4758,7 @@
         <v>784663</v>
       </c>
       <c r="K82" s="2" t="n">
-        <v>45395</v>
+        <v>45459</v>
       </c>
       <c r="L82" t="inlineStr">
         <is>
@@ -4811,7 +4811,7 @@
         <v>785466</v>
       </c>
       <c r="K83" s="2" t="n">
-        <v>45395</v>
+        <v>45459</v>
       </c>
       <c r="L83" t="inlineStr">
         <is>
@@ -4864,7 +4864,7 @@
         <v>784639</v>
       </c>
       <c r="K84" s="2" t="n">
-        <v>45395</v>
+        <v>45459</v>
       </c>
       <c r="L84" t="inlineStr">
         <is>
@@ -4917,7 +4917,7 @@
         <v>787735</v>
       </c>
       <c r="K85" s="2" t="n">
-        <v>45395</v>
+        <v>45459</v>
       </c>
       <c r="L85" t="inlineStr">
         <is>
@@ -4970,7 +4970,7 @@
         <v>786600</v>
       </c>
       <c r="K86" s="2" t="n">
-        <v>45395</v>
+        <v>45459</v>
       </c>
       <c r="L86" t="inlineStr">
         <is>
@@ -5023,7 +5023,7 @@
         <v>794590</v>
       </c>
       <c r="K87" s="2" t="n">
-        <v>45395</v>
+        <v>45459</v>
       </c>
       <c r="L87" t="inlineStr">
         <is>
@@ -5076,7 +5076,7 @@
         <v>801563</v>
       </c>
       <c r="K88" s="2" t="n">
-        <v>45395</v>
+        <v>45459</v>
       </c>
       <c r="L88" t="inlineStr">
         <is>
@@ -5129,7 +5129,7 @@
         <v>784709</v>
       </c>
       <c r="K89" s="2" t="n">
-        <v>45395</v>
+        <v>45460</v>
       </c>
       <c r="L89" t="inlineStr">
         <is>
@@ -5182,7 +5182,7 @@
         <v>791416</v>
       </c>
       <c r="K90" s="2" t="n">
-        <v>45395</v>
+        <v>45462</v>
       </c>
       <c r="L90" t="inlineStr">
         <is>
@@ -5235,7 +5235,7 @@
         <v>798839</v>
       </c>
       <c r="K91" s="2" t="n">
-        <v>45395</v>
+        <v>45462</v>
       </c>
       <c r="L91" t="inlineStr">
         <is>
@@ -5288,7 +5288,7 @@
         <v>787598</v>
       </c>
       <c r="K92" s="2" t="n">
-        <v>45395</v>
+        <v>45462</v>
       </c>
       <c r="L92" t="inlineStr">
         <is>
@@ -5341,7 +5341,7 @@
         <v>804981</v>
       </c>
       <c r="K93" s="2" t="n">
-        <v>45395</v>
+        <v>45462</v>
       </c>
       <c r="L93" t="inlineStr">
         <is>
@@ -5394,7 +5394,7 @@
         <v>5474</v>
       </c>
       <c r="K94" s="2" t="n">
-        <v>45395</v>
+        <v>45462</v>
       </c>
       <c r="L94" t="inlineStr">
         <is>
@@ -5447,7 +5447,7 @@
         <v>108391</v>
       </c>
       <c r="K95" s="2" t="n">
-        <v>45395</v>
+        <v>45462</v>
       </c>
       <c r="L95" t="inlineStr">
         <is>
@@ -5500,7 +5500,7 @@
         <v>802281</v>
       </c>
       <c r="K96" s="2" t="n">
-        <v>45395</v>
+        <v>45462</v>
       </c>
       <c r="L96" t="inlineStr">
         <is>
@@ -5553,7 +5553,7 @@
         <v>784886</v>
       </c>
       <c r="K97" s="2" t="n">
-        <v>45395</v>
+        <v>45463</v>
       </c>
       <c r="L97" t="inlineStr">
         <is>
@@ -5606,7 +5606,7 @@
         <v>787735</v>
       </c>
       <c r="K98" s="2" t="n">
-        <v>45395</v>
+        <v>45463</v>
       </c>
       <c r="L98" t="inlineStr">
         <is>
@@ -5659,7 +5659,7 @@
         <v>125341</v>
       </c>
       <c r="K99" s="2" t="n">
-        <v>45395</v>
+        <v>45463</v>
       </c>
       <c r="L99" t="inlineStr">
         <is>
@@ -5712,7 +5712,7 @@
         <v>794590</v>
       </c>
       <c r="K100" s="2" t="n">
-        <v>45395</v>
+        <v>45465</v>
       </c>
       <c r="L100" t="inlineStr">
         <is>
@@ -5765,7 +5765,7 @@
         <v>784639</v>
       </c>
       <c r="K101" s="2" t="n">
-        <v>45395</v>
+        <v>45465</v>
       </c>
       <c r="L101" t="inlineStr">
         <is>
@@ -5818,7 +5818,7 @@
         <v>797117</v>
       </c>
       <c r="K102" s="2" t="n">
-        <v>45395</v>
+        <v>45465</v>
       </c>
       <c r="L102" t="inlineStr">
         <is>
@@ -5871,7 +5871,7 @@
         <v>785466</v>
       </c>
       <c r="K103" s="2" t="n">
-        <v>45395</v>
+        <v>45465</v>
       </c>
       <c r="L103" t="inlineStr">
         <is>
@@ -5924,7 +5924,7 @@
         <v>802281</v>
       </c>
       <c r="K104" s="2" t="n">
-        <v>45395</v>
+        <v>45466</v>
       </c>
       <c r="L104" t="inlineStr">
         <is>
@@ -5977,7 +5977,7 @@
         <v>801563</v>
       </c>
       <c r="K105" s="2" t="n">
-        <v>45395</v>
+        <v>45466</v>
       </c>
       <c r="L105" t="inlineStr">
         <is>
@@ -6030,7 +6030,7 @@
         <v>784663</v>
       </c>
       <c r="K106" s="2" t="n">
-        <v>45395</v>
+        <v>45466</v>
       </c>
       <c r="L106" t="inlineStr">
         <is>
@@ -6083,7 +6083,7 @@
         <v>786600</v>
       </c>
       <c r="K107" s="2" t="n">
-        <v>45395</v>
+        <v>45466</v>
       </c>
       <c r="L107" t="inlineStr">
         <is>
@@ -6136,7 +6136,7 @@
         <v>784982</v>
       </c>
       <c r="K108" s="2" t="n">
-        <v>45395</v>
+        <v>45466</v>
       </c>
       <c r="L108" t="inlineStr">
         <is>
@@ -6189,7 +6189,7 @@
         <v>793051</v>
       </c>
       <c r="K109" s="2" t="n">
-        <v>45395</v>
+        <v>45466</v>
       </c>
       <c r="L109" t="inlineStr">
         <is>
@@ -6242,7 +6242,7 @@
         <v>125341</v>
       </c>
       <c r="K110" s="2" t="n">
-        <v>45395</v>
+        <v>45469</v>
       </c>
       <c r="L110" t="inlineStr">
         <is>
@@ -6295,7 +6295,7 @@
         <v>798839</v>
       </c>
       <c r="K111" s="2" t="n">
-        <v>45395</v>
+        <v>45469</v>
       </c>
       <c r="L111" t="inlineStr">
         <is>
@@ -6348,7 +6348,7 @@
         <v>787598</v>
       </c>
       <c r="K112" s="2" t="n">
-        <v>45395</v>
+        <v>45469</v>
       </c>
       <c r="L112" t="inlineStr">
         <is>
@@ -6401,7 +6401,7 @@
         <v>5474</v>
       </c>
       <c r="K113" s="2" t="n">
-        <v>45395</v>
+        <v>45469</v>
       </c>
       <c r="L113" t="inlineStr">
         <is>
@@ -6454,7 +6454,7 @@
         <v>784663</v>
       </c>
       <c r="K114" s="2" t="n">
-        <v>45395</v>
+        <v>45469</v>
       </c>
       <c r="L114" t="inlineStr">
         <is>
@@ -6507,7 +6507,7 @@
         <v>804981</v>
       </c>
       <c r="K115" s="2" t="n">
-        <v>45395</v>
+        <v>45469</v>
       </c>
       <c r="L115" t="inlineStr">
         <is>
@@ -6560,7 +6560,7 @@
         <v>784709</v>
       </c>
       <c r="K116" s="2" t="n">
-        <v>45395</v>
+        <v>45469</v>
       </c>
       <c r="L116" t="inlineStr">
         <is>
@@ -6613,7 +6613,7 @@
         <v>784886</v>
       </c>
       <c r="K117" s="2" t="n">
-        <v>45395</v>
+        <v>45469</v>
       </c>
       <c r="L117" t="inlineStr">
         <is>
@@ -6666,7 +6666,7 @@
         <v>793051</v>
       </c>
       <c r="K118" s="2" t="n">
-        <v>45395</v>
+        <v>45470</v>
       </c>
       <c r="L118" t="inlineStr">
         <is>
@@ -6719,7 +6719,7 @@
         <v>791416</v>
       </c>
       <c r="K119" s="2" t="n">
-        <v>45395</v>
+        <v>45470</v>
       </c>
       <c r="L119" t="inlineStr">
         <is>
@@ -6772,7 +6772,7 @@
         <v>125341</v>
       </c>
       <c r="K120" s="2" t="n">
-        <v>45395</v>
+        <v>45472</v>
       </c>
       <c r="L120" t="inlineStr">
         <is>
@@ -6825,7 +6825,7 @@
         <v>794590</v>
       </c>
       <c r="K121" s="2" t="n">
-        <v>45395</v>
+        <v>45472</v>
       </c>
       <c r="L121" t="inlineStr">
         <is>
@@ -6878,7 +6878,7 @@
         <v>797117</v>
       </c>
       <c r="K122" s="2" t="n">
-        <v>45395</v>
+        <v>45473</v>
       </c>
       <c r="L122" t="inlineStr">
         <is>
@@ -6931,7 +6931,7 @@
         <v>784982</v>
       </c>
       <c r="K123" s="2" t="n">
-        <v>45395</v>
+        <v>45473</v>
       </c>
       <c r="L123" t="inlineStr">
         <is>
@@ -6984,7 +6984,7 @@
         <v>108391</v>
       </c>
       <c r="K124" s="2" t="n">
-        <v>45395</v>
+        <v>45473</v>
       </c>
       <c r="L124" t="inlineStr">
         <is>
@@ -7037,7 +7037,7 @@
         <v>787735</v>
       </c>
       <c r="K125" s="2" t="n">
-        <v>45395</v>
+        <v>45473</v>
       </c>
       <c r="L125" t="inlineStr">
         <is>
@@ -7090,7 +7090,7 @@
         <v>784639</v>
       </c>
       <c r="K126" s="2" t="n">
-        <v>45395</v>
+        <v>45473</v>
       </c>
       <c r="L126" t="inlineStr">
         <is>
@@ -7143,7 +7143,7 @@
         <v>801563</v>
       </c>
       <c r="K127" s="2" t="n">
-        <v>45395</v>
+        <v>45473</v>
       </c>
       <c r="L127" t="inlineStr">
         <is>
@@ -7196,7 +7196,7 @@
         <v>798839</v>
       </c>
       <c r="K128" s="2" t="n">
-        <v>45395</v>
+        <v>45473</v>
       </c>
       <c r="L128" t="inlineStr">
         <is>
@@ -7249,7 +7249,7 @@
         <v>802281</v>
       </c>
       <c r="K129" s="2" t="n">
-        <v>45395</v>
+        <v>45474</v>
       </c>
       <c r="L129" t="inlineStr">
         <is>
@@ -7302,7 +7302,7 @@
         <v>794590</v>
       </c>
       <c r="K130" s="2" t="n">
-        <v>45395</v>
+        <v>45476</v>
       </c>
       <c r="L130" t="inlineStr">
         <is>
@@ -7355,7 +7355,7 @@
         <v>801563</v>
       </c>
       <c r="K131" s="2" t="n">
-        <v>45395</v>
+        <v>45476</v>
       </c>
       <c r="L131" t="inlineStr">
         <is>
@@ -7408,7 +7408,7 @@
         <v>786600</v>
       </c>
       <c r="K132" s="2" t="n">
-        <v>45395</v>
+        <v>45476</v>
       </c>
       <c r="L132" t="inlineStr">
         <is>
@@ -7461,7 +7461,7 @@
         <v>785466</v>
       </c>
       <c r="K133" s="2" t="n">
-        <v>45395</v>
+        <v>45476</v>
       </c>
       <c r="L133" t="inlineStr">
         <is>
@@ -7514,7 +7514,7 @@
         <v>784663</v>
       </c>
       <c r="K134" s="2" t="n">
-        <v>45395</v>
+        <v>45476</v>
       </c>
       <c r="L134" t="inlineStr">
         <is>
@@ -7567,7 +7567,7 @@
         <v>797117</v>
       </c>
       <c r="K135" s="2" t="n">
-        <v>45395</v>
+        <v>45476</v>
       </c>
       <c r="L135" t="inlineStr">
         <is>
@@ -7620,7 +7620,7 @@
         <v>784982</v>
       </c>
       <c r="K136" s="2" t="n">
-        <v>45395</v>
+        <v>45477</v>
       </c>
       <c r="L136" t="inlineStr">
         <is>
@@ -7673,7 +7673,7 @@
         <v>784709</v>
       </c>
       <c r="K137" s="2" t="n">
-        <v>45395</v>
+        <v>45477</v>
       </c>
       <c r="L137" t="inlineStr">
         <is>
@@ -7726,7 +7726,7 @@
         <v>793051</v>
       </c>
       <c r="K138" s="2" t="n">
-        <v>45395</v>
+        <v>45477</v>
       </c>
       <c r="L138" t="inlineStr">
         <is>
@@ -7779,7 +7779,7 @@
         <v>784639</v>
       </c>
       <c r="K139" s="2" t="n">
-        <v>45395</v>
+        <v>45477</v>
       </c>
       <c r="L139" t="inlineStr">
         <is>
@@ -7832,7 +7832,7 @@
         <v>5474</v>
       </c>
       <c r="K140" s="2" t="n">
-        <v>45395</v>
+        <v>45479</v>
       </c>
       <c r="L140" t="inlineStr">
         <is>
@@ -7885,7 +7885,7 @@
         <v>125341</v>
       </c>
       <c r="K141" s="2" t="n">
-        <v>45395</v>
+        <v>45479</v>
       </c>
       <c r="L141" t="inlineStr">
         <is>
@@ -7938,7 +7938,7 @@
         <v>802281</v>
       </c>
       <c r="K142" s="2" t="n">
-        <v>45395</v>
+        <v>45480</v>
       </c>
       <c r="L142" t="inlineStr">
         <is>
@@ -7991,7 +7991,7 @@
         <v>108391</v>
       </c>
       <c r="K143" s="2" t="n">
-        <v>45395</v>
+        <v>45480</v>
       </c>
       <c r="L143" t="inlineStr">
         <is>
@@ -8044,7 +8044,7 @@
         <v>787598</v>
       </c>
       <c r="K144" s="2" t="n">
-        <v>45395</v>
+        <v>45480</v>
       </c>
       <c r="L144" t="inlineStr">
         <is>
@@ -8097,7 +8097,7 @@
         <v>804981</v>
       </c>
       <c r="K145" s="2" t="n">
-        <v>45395</v>
+        <v>45480</v>
       </c>
       <c r="L145" t="inlineStr">
         <is>
@@ -8150,7 +8150,7 @@
         <v>798839</v>
       </c>
       <c r="K146" s="2" t="n">
-        <v>45395</v>
+        <v>45480</v>
       </c>
       <c r="L146" t="inlineStr">
         <is>
@@ -8203,7 +8203,7 @@
         <v>787735</v>
       </c>
       <c r="K147" s="2" t="n">
-        <v>45395</v>
+        <v>45480</v>
       </c>
       <c r="L147" t="inlineStr">
         <is>
@@ -8256,7 +8256,7 @@
         <v>791416</v>
       </c>
       <c r="K148" s="2" t="n">
-        <v>45395</v>
+        <v>45480</v>
       </c>
       <c r="L148" t="inlineStr">
         <is>
@@ -8309,7 +8309,7 @@
         <v>784886</v>
       </c>
       <c r="K149" s="2" t="n">
-        <v>45395</v>
+        <v>45480</v>
       </c>
       <c r="L149" t="inlineStr">
         <is>
@@ -8405,7 +8405,7 @@
         <v>801563</v>
       </c>
       <c r="K151" s="2" t="n">
-        <v>45395</v>
+        <v>45483</v>
       </c>
       <c r="L151" t="inlineStr">
         <is>
@@ -8458,7 +8458,7 @@
         <v>787735</v>
       </c>
       <c r="K152" s="2" t="n">
-        <v>45395</v>
+        <v>45483</v>
       </c>
       <c r="L152" t="inlineStr">
         <is>
@@ -8554,7 +8554,7 @@
         <v>802281</v>
       </c>
       <c r="K154" s="2" t="n">
-        <v>45395</v>
+        <v>45483</v>
       </c>
       <c r="L154" t="inlineStr">
         <is>
@@ -8607,7 +8607,7 @@
         <v>164969</v>
       </c>
       <c r="K155" s="2" t="n">
-        <v>45395</v>
+        <v>45484</v>
       </c>
       <c r="L155" t="inlineStr">
         <is>
@@ -8660,7 +8660,7 @@
         <v>108391</v>
       </c>
       <c r="K156" s="2" t="n">
-        <v>45395</v>
+        <v>45484</v>
       </c>
       <c r="L156" t="inlineStr">
         <is>
@@ -8713,7 +8713,7 @@
         <v>786600</v>
       </c>
       <c r="K157" s="2" t="n">
-        <v>45395</v>
+        <v>45484</v>
       </c>
       <c r="L157" t="inlineStr">
         <is>
@@ -8766,7 +8766,7 @@
         <v>785466</v>
       </c>
       <c r="K158" s="2" t="n">
-        <v>45395</v>
+        <v>45484</v>
       </c>
       <c r="L158" t="inlineStr">
         <is>
@@ -8819,7 +8819,7 @@
         <v>794590</v>
       </c>
       <c r="K159" s="2" t="n">
-        <v>45395</v>
+        <v>45484</v>
       </c>
       <c r="L159" t="inlineStr">
         <is>

</xml_diff>

<commit_message>
Atualizações dados 17/07 19h
</commit_message>
<xml_diff>
--- a/data/matches.xlsx
+++ b/data/matches.xlsx
@@ -1181,7 +1181,7 @@
       <c r="N13" t="inlineStr"/>
       <c r="O13" t="inlineStr"/>
       <c r="P13" s="3" t="n">
-        <v>45490.00259259259</v>
+        <v>45490.81285879629</v>
       </c>
     </row>
     <row r="14">
@@ -1731,7 +1731,7 @@
       <c r="N23" t="inlineStr"/>
       <c r="O23" t="inlineStr"/>
       <c r="P23" s="3" t="n">
-        <v>45490.00259259259</v>
+        <v>45490.81285879629</v>
       </c>
     </row>
     <row r="24">
@@ -2281,7 +2281,7 @@
       <c r="N33" t="inlineStr"/>
       <c r="O33" t="inlineStr"/>
       <c r="P33" s="3" t="n">
-        <v>45490.00259259259</v>
+        <v>45490.81285879629</v>
       </c>
     </row>
     <row r="34">
@@ -8808,7 +8808,7 @@
       <c r="I150" t="inlineStr"/>
       <c r="J150" t="inlineStr"/>
       <c r="K150" s="2" t="n">
-        <v>45483</v>
+        <v>45482</v>
       </c>
       <c r="L150" t="inlineStr">
         <is>
@@ -8823,7 +8823,7 @@
       <c r="N150" t="inlineStr"/>
       <c r="O150" t="inlineStr"/>
       <c r="P150" s="3" t="n">
-        <v>45490.00259259259</v>
+        <v>45490.81285879629</v>
       </c>
     </row>
     <row r="151">
@@ -8981,7 +8981,7 @@
       <c r="N153" t="inlineStr"/>
       <c r="O153" t="inlineStr"/>
       <c r="P153" s="3" t="n">
-        <v>45490.00259259259</v>
+        <v>45490.81285879629</v>
       </c>
     </row>
     <row r="154">
@@ -9531,7 +9531,7 @@
       <c r="N163" t="inlineStr"/>
       <c r="O163" t="inlineStr"/>
       <c r="P163" s="3" t="n">
-        <v>45490.00259259259</v>
+        <v>45490.81285879629</v>
       </c>
     </row>
     <row r="164">
@@ -9577,7 +9577,7 @@
       <c r="N164" t="inlineStr"/>
       <c r="O164" t="inlineStr"/>
       <c r="P164" s="3" t="n">
-        <v>45490.00260416666</v>
+        <v>45490.81285879629</v>
       </c>
     </row>
     <row r="165">
@@ -9601,7 +9601,7 @@
       </c>
       <c r="G165" t="inlineStr">
         <is>
-          <t>notstarted</t>
+          <t>inprogress</t>
         </is>
       </c>
       <c r="H165" t="inlineStr"/>
@@ -9623,7 +9623,7 @@
       <c r="N165" t="inlineStr"/>
       <c r="O165" t="inlineStr"/>
       <c r="P165" s="3" t="n">
-        <v>45490.00260416666</v>
+        <v>45490.81285879629</v>
       </c>
     </row>
     <row r="166">
@@ -9669,7 +9669,7 @@
       <c r="N166" t="inlineStr"/>
       <c r="O166" t="inlineStr"/>
       <c r="P166" s="3" t="n">
-        <v>45490.00260416666</v>
+        <v>45490.81285879629</v>
       </c>
     </row>
     <row r="167">
@@ -9715,7 +9715,7 @@
       <c r="N167" t="inlineStr"/>
       <c r="O167" t="inlineStr"/>
       <c r="P167" s="3" t="n">
-        <v>45490.00260416666</v>
+        <v>45490.81285879629</v>
       </c>
     </row>
     <row r="168">
@@ -9761,7 +9761,7 @@
       <c r="N168" t="inlineStr"/>
       <c r="O168" t="inlineStr"/>
       <c r="P168" s="3" t="n">
-        <v>45490.00260416666</v>
+        <v>45490.81285879629</v>
       </c>
     </row>
     <row r="169">

</xml_diff>

<commit_message>
Atualizações dados 19/07 19h
</commit_message>
<xml_diff>
--- a/data/matches.xlsx
+++ b/data/matches.xlsx
@@ -1311,7 +1311,7 @@
       <c r="P13" t="inlineStr"/>
       <c r="Q13" t="inlineStr"/>
       <c r="R13" s="3" t="n">
-        <v>45492.67011574074</v>
+        <v>45492.81358796296</v>
       </c>
     </row>
     <row r="14">
@@ -1961,7 +1961,7 @@
       <c r="P23" t="inlineStr"/>
       <c r="Q23" t="inlineStr"/>
       <c r="R23" s="3" t="n">
-        <v>45492.67011574074</v>
+        <v>45492.81358796296</v>
       </c>
     </row>
     <row r="24">
@@ -2611,7 +2611,7 @@
       <c r="P33" t="inlineStr"/>
       <c r="Q33" t="inlineStr"/>
       <c r="R33" s="3" t="n">
-        <v>45492.67011574074</v>
+        <v>45492.81358796296</v>
       </c>
     </row>
     <row r="34">
@@ -10323,7 +10323,7 @@
       <c r="P150" t="inlineStr"/>
       <c r="Q150" t="inlineStr"/>
       <c r="R150" s="3" t="n">
-        <v>45492.67011574074</v>
+        <v>45492.81358796296</v>
       </c>
     </row>
     <row r="151">
@@ -10511,7 +10511,7 @@
       <c r="P153" t="inlineStr"/>
       <c r="Q153" t="inlineStr"/>
       <c r="R153" s="3" t="n">
-        <v>45492.67011574074</v>
+        <v>45492.81358796296</v>
       </c>
     </row>
     <row r="154">
@@ -11227,7 +11227,7 @@
       <c r="P164" t="inlineStr"/>
       <c r="Q164" t="inlineStr"/>
       <c r="R164" s="3" t="n">
-        <v>45492.67011574074</v>
+        <v>45492.81358796296</v>
       </c>
     </row>
     <row r="165">
@@ -11283,7 +11283,7 @@
       <c r="P165" t="inlineStr"/>
       <c r="Q165" t="inlineStr"/>
       <c r="R165" s="3" t="n">
-        <v>45492.67011574074</v>
+        <v>45492.81358796296</v>
       </c>
     </row>
     <row r="166">
@@ -11603,7 +11603,7 @@
       <c r="P170" t="inlineStr"/>
       <c r="Q170" t="inlineStr"/>
       <c r="R170" s="3" t="n">
-        <v>45492.67011574074</v>
+        <v>45492.81358796296</v>
       </c>
     </row>
     <row r="171">
@@ -11659,7 +11659,7 @@
       <c r="P171" t="inlineStr"/>
       <c r="Q171" t="inlineStr"/>
       <c r="R171" s="3" t="n">
-        <v>45492.67011574074</v>
+        <v>45492.81358796296</v>
       </c>
     </row>
     <row r="172">
@@ -11715,7 +11715,7 @@
       <c r="P172" t="inlineStr"/>
       <c r="Q172" t="inlineStr"/>
       <c r="R172" s="3" t="n">
-        <v>45492.67011574074</v>
+        <v>45492.81358796296</v>
       </c>
     </row>
     <row r="173">
@@ -11771,7 +11771,7 @@
       <c r="P173" t="inlineStr"/>
       <c r="Q173" t="inlineStr"/>
       <c r="R173" s="3" t="n">
-        <v>45492.67011574074</v>
+        <v>45492.81358796296</v>
       </c>
     </row>
     <row r="174">
@@ -11827,7 +11827,7 @@
       <c r="P174" t="inlineStr"/>
       <c r="Q174" t="inlineStr"/>
       <c r="R174" s="3" t="n">
-        <v>45492.67011574074</v>
+        <v>45492.81358796296</v>
       </c>
     </row>
     <row r="175">
@@ -11883,7 +11883,7 @@
       <c r="P175" t="inlineStr"/>
       <c r="Q175" t="inlineStr"/>
       <c r="R175" s="3" t="n">
-        <v>45492.67011574074</v>
+        <v>45492.81358796296</v>
       </c>
     </row>
     <row r="176">
@@ -11939,7 +11939,7 @@
       <c r="P176" t="inlineStr"/>
       <c r="Q176" t="inlineStr"/>
       <c r="R176" s="3" t="n">
-        <v>45492.67011574074</v>
+        <v>45492.81358796296</v>
       </c>
     </row>
     <row r="177">
@@ -11995,7 +11995,7 @@
       <c r="P177" t="inlineStr"/>
       <c r="Q177" t="inlineStr"/>
       <c r="R177" s="3" t="n">
-        <v>45492.67011574074</v>
+        <v>45492.81358796296</v>
       </c>
     </row>
     <row r="178">
@@ -12051,7 +12051,7 @@
       <c r="P178" t="inlineStr"/>
       <c r="Q178" t="inlineStr"/>
       <c r="R178" s="3" t="n">
-        <v>45492.67011574074</v>
+        <v>45492.81358796296</v>
       </c>
     </row>
     <row r="179">
@@ -12107,7 +12107,7 @@
       <c r="P179" t="inlineStr"/>
       <c r="Q179" t="inlineStr"/>
       <c r="R179" s="3" t="n">
-        <v>45492.67011574074</v>
+        <v>45492.81358796296</v>
       </c>
     </row>
   </sheetData>

</xml_diff>